<commit_message>
Update Stock Modeling Results.xlsx
</commit_message>
<xml_diff>
--- a/04_Stock_Modeling/Stock Modeling Results.xlsx
+++ b/04_Stock_Modeling/Stock Modeling Results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1351d315c21e3c97/Documents/Rice/Summer Semester/Capstone/Project/CVX_Rice_project/04_Stock_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="11_F25DC773A252ABDACC10487521D870CC5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{756EB816-9DF6-4863-B8F8-BCF932DB16C8}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="11_F25DC773A252ABDACC10487521D870CC5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{612020D9-09E7-4A3D-91DC-84D166803584}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$61</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="34">
   <si>
     <t>Sentiment Source</t>
   </si>
@@ -109,13 +110,34 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Early Learnings</t>
+  </si>
+  <si>
+    <t>Random Forest has the best results from a model perspective</t>
+  </si>
+  <si>
+    <t>Next Steps</t>
+  </si>
+  <si>
+    <t>4 - Test different model combinations on Best Model</t>
+  </si>
+  <si>
+    <t>3 - Date cutoffs on Best Model</t>
+  </si>
+  <si>
+    <t>2 - Test SMOTE on Best Model</t>
+  </si>
+  <si>
+    <t>1 - Tune all existing random forest models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +149,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -187,11 +222,31 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -471,11 +526,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -490,7 +546,7 @@
     <col min="10" max="10" width="46.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,31 +568,25 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="E2" s="11"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -556,11 +606,8 @@
         <v>26</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -580,11 +627,8 @@
         <v>26</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -604,11 +648,8 @@
         <v>26</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -629,24 +670,24 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -663,75 +704,75 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="B10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A11" s="4" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="B11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="E12" s="15"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -752,7 +793,7 @@
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -773,7 +814,7 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -794,7 +835,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
@@ -815,22 +856,22 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="8" t="s">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="8" t="s">
@@ -853,7 +894,7 @@
       </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
@@ -874,7 +915,7 @@
       </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
@@ -895,7 +936,7 @@
       </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -916,22 +957,22 @@
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="6" t="s">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" s="6" t="s">
@@ -954,7 +995,7 @@
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A24" s="6" t="s">
         <v>13</v>
       </c>
@@ -975,7 +1016,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
@@ -996,7 +1037,7 @@
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A26" s="6" t="s">
         <v>13</v>
       </c>
@@ -1017,22 +1058,22 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="8" t="s">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" s="8" t="s">
@@ -1047,62 +1088,78 @@
       <c r="D28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8"/>
+      <c r="E28" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A29" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="8" t="s">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="E29" s="20">
+        <v>0.49</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="E30" s="20">
+        <v>0.47</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E31" s="20">
+        <v>0.51</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1201,7 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1222,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1186,7 +1243,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1207,22 +1264,22 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="B37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A38" s="4" t="s">
@@ -1241,158 +1298,158 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="B39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A40" s="4" t="s">
+      <c r="E39" s="13"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="B40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A41" s="4" t="s">
+      <c r="E40" s="13"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="B41" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="E41" s="13"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="E42" s="15"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="6" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="E45" s="15"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="E46" s="15"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A48" s="8" t="s">
@@ -1411,58 +1468,58 @@
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A49" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="8" t="s">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A49" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="8" t="s">
+      <c r="E49" s="17"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A50" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="9"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A51" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="8" t="s">
+      <c r="E50" s="17"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E51" s="17"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A52" s="6" t="s">
         <v>13</v>
       </c>
@@ -1504,7 +1561,7 @@
       </c>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A54" s="6" t="s">
         <v>13</v>
       </c>
@@ -1525,7 +1582,7 @@
       </c>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A55" s="6" t="s">
         <v>13</v>
       </c>
@@ -1546,7 +1603,7 @@
       </c>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A56" s="6" t="s">
         <v>13</v>
       </c>
@@ -1567,7 +1624,7 @@
       </c>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A57" s="8" t="s">
         <v>15</v>
       </c>
@@ -1609,7 +1666,7 @@
       </c>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A59" s="8" t="s">
         <v>15</v>
       </c>
@@ -1630,7 +1687,7 @@
       </c>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A60" s="8" t="s">
         <v>15</v>
       </c>
@@ -1651,7 +1708,7 @@
       </c>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A61" s="8" t="s">
         <v>15</v>
       </c>
@@ -1672,9 +1729,105 @@
       </c>
       <c r="G61" s="8"/>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G61" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G61" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0" cellColor="0"/>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Random Forest"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9562F26E-E026-4B2F-AD21-5AF3E6E201D0}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="49.234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Move Files_update stock model excel
Organized notebooks and updated excel file for stock model results
</commit_message>
<xml_diff>
--- a/04_Stock_Modeling/Stock Modeling Results.xlsx
+++ b/04_Stock_Modeling/Stock Modeling Results.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlattal/Documents/GitHub/CVX_Rice_project/04_Stock_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BBC12F-4C95-0E46-A39D-5E560B7DD3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3B21FE-FBCA-2F4D-8434-534A8B3343DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1060" windowWidth="33820" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1040" windowWidth="33820" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$89</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="52">
   <si>
     <t>Sentiment Source</t>
   </si>
@@ -574,11 +574,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1911,22 +1911,24 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="19">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F68" s="8"/>
+      <c r="A68" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="G68" s="8" t="s">
         <v>51</v>
       </c>
@@ -1942,10 +1944,10 @@
         <v>22</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E69" s="19">
-        <v>0.55000000000000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="8" t="s">
@@ -1963,10 +1965,10 @@
         <v>22</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E70" s="19">
-        <v>0.54</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8" t="s">
@@ -1974,61 +1976,65 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D71" s="16" t="s">
+      <c r="A71" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="19">
+        <v>0.54</v>
+      </c>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D72" s="8" t="s">
+      <c r="E72" s="17"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E72" s="9">
+      <c r="E73" s="9">
         <v>0.62</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F73" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G72" s="20" t="s">
+      <c r="G73" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="17"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
@@ -2041,7 +2047,7 @@
         <v>23</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E74" s="17"/>
       <c r="F74" s="16"/>
@@ -2058,32 +2064,28 @@
         <v>23</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E75" s="17"/>
       <c r="F75" s="16"/>
       <c r="G75" s="16"/>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="7">
-        <v>0.53</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G76" s="6"/>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="17"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
     </row>
     <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
@@ -2096,17 +2098,15 @@
         <v>23</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E77" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G77" s="6"/>
     </row>
     <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
@@ -2119,15 +2119,17 @@
         <v>23</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78" s="7">
-        <v>0.52</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G78" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
@@ -2140,10 +2142,10 @@
         <v>23</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E79" s="7">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>25</v>
@@ -2161,7 +2163,7 @@
         <v>23</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E80" s="7">
         <v>0.51</v>
@@ -2171,26 +2173,26 @@
       </c>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="9">
-        <v>0.49</v>
-      </c>
-      <c r="F81" s="8" t="s">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="F81" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G81" s="8"/>
+      <c r="G81" s="6"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
@@ -2203,17 +2205,15 @@
         <v>23</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E82" s="9">
-        <v>0.55000000000000004</v>
+        <v>0.49</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G82" s="20" t="s">
-        <v>42</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G82" s="8"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
@@ -2226,15 +2226,17 @@
         <v>23</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E83" s="9">
-        <v>0.49</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
@@ -2247,10 +2249,10 @@
         <v>23</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E84" s="9">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>25</v>
@@ -2268,10 +2270,10 @@
         <v>23</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E85" s="9">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>25</v>
@@ -2283,30 +2285,28 @@
         <v>15</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="17">
-        <v>0.62</v>
+        <v>12</v>
+      </c>
+      <c r="E86" s="9">
+        <v>0.54</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G86" s="16" t="s">
-        <v>46</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G86" s="8"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>23</v>
@@ -2314,14 +2314,14 @@
       <c r="D87" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E87" s="9">
-        <v>0.55000000000000004</v>
+      <c r="E87" s="17">
+        <v>0.62</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G87" s="20" t="s">
-        <v>45</v>
+      <c r="G87" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2329,7 +2329,7 @@
         <v>15</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>23</v>
@@ -2338,17 +2338,40 @@
         <v>9</v>
       </c>
       <c r="E88" s="9">
-        <v>0.53</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F88" s="8" t="s">
         <v>44</v>
       </c>
       <c r="G88" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G89" s="20" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G88" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:G89" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Gemini Prompt2"/>

</xml_diff>

<commit_message>
aggregated stock model updates
added various stock model tuning updates. updated stock modeling results excel
</commit_message>
<xml_diff>
--- a/04_Stock_Modeling/Stock Modeling Results.xlsx
+++ b/04_Stock_Modeling/Stock Modeling Results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlattal/Documents/GitHub/CVX_Rice_project/04_Stock_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3B21FE-FBCA-2F4D-8434-534A8B3343DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D822189-DD8B-E640-A30E-C134D8568CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1040" windowWidth="33820" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22040" yWindow="500" windowWidth="22040" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$90</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="56">
   <si>
     <t>Sentiment Source</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>Added weekly returns to features</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Changed split to (Train: 2021-2023 / Test: 2023-current) {'n_estimators': 20} {'max_depth': 20} {'max_features': 0.8} {'min_samples_split': 4} {'min_samples_leaf': 7}</t>
+  </si>
+  <si>
+    <t>All (excl PQ)</t>
+  </si>
+  <si>
+    <t>split to (Train: 2022-2024 / Test: 2024-current)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Changed split to (Train: 2021-2023 / Test: 2023-current) Best parameters found:  {'C': 0.1, 'gamma': 'auto', 'kernel': 'sigmoid'}</t>
   </si>
 </sst>
 </file>
@@ -574,11 +586,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -941,7 +953,9 @@
       <c r="F18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -1374,33 +1388,37 @@
         <v>9</v>
       </c>
       <c r="E40" s="9">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G40" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="19">
-        <v>0.49</v>
+      <c r="A41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="9">
+        <v>0.54</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
@@ -1413,10 +1431,10 @@
         <v>22</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" s="19">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>26</v>
@@ -1434,36 +1452,36 @@
         <v>22</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E43" s="19">
-        <v>0.51</v>
+        <v>0.47</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G43" s="18"/>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0.46</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="2"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="19">
+        <v>0.51</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
@@ -1476,17 +1494,15 @@
         <v>23</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E45" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.46</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -1499,15 +1515,17 @@
         <v>23</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46" s="3">
-        <v>0.51</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -1520,10 +1538,10 @@
         <v>23</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E47" s="3">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>25</v>
@@ -1541,7 +1559,7 @@
         <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E48" s="3">
         <v>0.5</v>
@@ -1552,55 +1570,59 @@
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="12" t="s">
+      <c r="B50" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="E50" s="13"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="B51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
@@ -1613,7 +1635,7 @@
         <v>23</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E52" s="13"/>
       <c r="F52" s="12"/>
@@ -1630,28 +1652,28 @@
         <v>23</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E53" s="13"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
     </row>
     <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="15"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
+      <c r="A54" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="13"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
     </row>
     <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
@@ -1664,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="14"/>
@@ -1681,7 +1703,7 @@
         <v>23</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="14"/>
@@ -1698,7 +1720,7 @@
         <v>23</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="14"/>
@@ -1715,47 +1737,43 @@
         <v>23</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E58" s="15"/>
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="8" t="s">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="15"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="19">
+      <c r="E60" s="9">
         <v>0.5</v>
       </c>
       <c r="F60" s="8"/>
@@ -1774,10 +1792,10 @@
         <v>22</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E61" s="19">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F61" s="8"/>
       <c r="G61" s="8" t="s">
@@ -1795,10 +1813,10 @@
         <v>22</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E62" s="19">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="8" t="s">
@@ -1806,41 +1824,41 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="9">
-        <v>0.52</v>
+      <c r="A63" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="19">
+        <v>0.48</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="19">
-        <v>0.51</v>
+      <c r="A64" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="9">
+        <v>0.52</v>
       </c>
       <c r="F64" s="8"/>
       <c r="G64" s="8" t="s">
@@ -1858,10 +1876,10 @@
         <v>22</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E65" s="19">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="8" t="s">
@@ -1879,10 +1897,10 @@
         <v>22</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E66" s="19">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8" t="s">
@@ -1890,24 +1908,24 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="9">
-        <v>0.56000000000000005</v>
+      <c r="A67" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="19">
+        <v>0.53</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -1924,32 +1942,32 @@
         <v>9</v>
       </c>
       <c r="E68" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>38</v>
-      </c>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F68" s="8"/>
       <c r="G68" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="19">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F69" s="8"/>
+      <c r="A69" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="G69" s="8" t="s">
         <v>51</v>
       </c>
@@ -1965,10 +1983,10 @@
         <v>22</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E70" s="19">
-        <v>0.55000000000000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8" t="s">
@@ -1986,10 +2004,10 @@
         <v>22</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E71" s="19">
-        <v>0.54</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="8" t="s">
@@ -1997,61 +2015,65 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D72" s="16" t="s">
+      <c r="A72" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="19">
+        <v>0.54</v>
+      </c>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E72" s="17"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D73" s="8" t="s">
+      <c r="E73" s="17"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E74" s="9">
         <v>0.62</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F74" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G73" s="20" t="s">
+      <c r="G74" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B74" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D74" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="17"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
@@ -2064,7 +2086,7 @@
         <v>23</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E75" s="17"/>
       <c r="F75" s="16"/>
@@ -2081,32 +2103,28 @@
         <v>23</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E76" s="17"/>
       <c r="F76" s="16"/>
       <c r="G76" s="16"/>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E77" s="7">
-        <v>0.53</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G77" s="6"/>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="17"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
     </row>
     <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
@@ -2119,17 +2137,15 @@
         <v>23</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E78" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G78" s="6"/>
     </row>
     <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
@@ -2142,15 +2158,17 @@
         <v>23</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E79" s="7">
-        <v>0.52</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
@@ -2163,10 +2181,10 @@
         <v>23</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E80" s="7">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>25</v>
@@ -2184,7 +2202,7 @@
         <v>23</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E81" s="7">
         <v>0.51</v>
@@ -2194,26 +2212,26 @@
       </c>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" s="9">
-        <v>0.49</v>
-      </c>
-      <c r="F82" s="8" t="s">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="F82" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G82" s="8"/>
+      <c r="G82" s="6"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
@@ -2226,17 +2244,15 @@
         <v>23</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E83" s="9">
-        <v>0.55000000000000004</v>
+        <v>0.49</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G83" s="20" t="s">
-        <v>42</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G83" s="8"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
@@ -2249,15 +2265,17 @@
         <v>23</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84" s="9">
-        <v>0.49</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G84" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
@@ -2270,10 +2288,10 @@
         <v>23</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E85" s="9">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>25</v>
@@ -2291,10 +2309,10 @@
         <v>23</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E86" s="9">
-        <v>0.54</v>
+        <v>0.51</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>25</v>
@@ -2306,30 +2324,28 @@
         <v>15</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="17">
-        <v>0.62</v>
+        <v>12</v>
+      </c>
+      <c r="E87" s="9">
+        <v>0.54</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G87" s="16" t="s">
-        <v>46</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G87" s="8"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>23</v>
@@ -2337,14 +2353,14 @@
       <c r="D88" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E88" s="9">
-        <v>0.55000000000000004</v>
+      <c r="E88" s="17">
+        <v>0.62</v>
       </c>
       <c r="F88" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G88" s="20" t="s">
-        <v>45</v>
+      <c r="G88" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2352,7 +2368,7 @@
         <v>15</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>23</v>
@@ -2361,17 +2377,40 @@
         <v>9</v>
       </c>
       <c r="E89" s="9">
-        <v>0.53</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>44</v>
       </c>
       <c r="G89" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G90" s="20" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G89" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:G90" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Gemini Prompt2"/>

</xml_diff>